<commit_message>
Modificação no arquivo indice+corresp+duas+condi
</commit_message>
<xml_diff>
--- a/Formulas importantes/Indice+Corresp+duas+Condições.xlsx
+++ b/Formulas importantes/Indice+Corresp+duas+Condições.xlsx
@@ -1,28 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Indice Corresp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Excel\Formulas importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D90C4E-C683-4DB4-9D5C-C140F69A4DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DEB906-592B-47F5-8933-B3E6D5D3ECA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D135085-162F-4F6A-83EE-95534B59CC74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1D135085-162F-4F6A-83EE-95534B59CC74}"/>
   </bookViews>
   <sheets>
     <sheet name="Professor" sheetId="1" r:id="rId1"/>
     <sheet name="Aluno" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,271 +571,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A096B3F-3F20-4D87-A3FB-7004DAEFE5F0}">
   <dimension ref="B2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I3" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="array" ref="D7">INDEX($I$7:$K$21,MATCH(B7&amp;C7,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
-        <v>89.99</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="10">
-        <v>89.99</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="array" ref="D8">INDEX($I$7:$K$21,MATCH(B8&amp;C8,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
-        <v>148.56</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="10">
-        <v>69.989999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="array" ref="D9">INDEX($I$7:$K$21,MATCH(B9&amp;C9,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
-        <v>46.9</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="10">
-        <v>153.4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="array" ref="D10">INDEX($I$7:$K$21,MATCH(B10&amp;C10,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
-        <v>69.989999999999995</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="10">
-        <v>148.56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="10">
-        <v>146.13999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="10">
-        <v>224.14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="10">
-        <v>150.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="10">
-        <v>248.73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="10">
-        <v>116.52</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="10">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="10">
-        <v>46.9</v>
-      </c>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="10">
-        <v>41.9</v>
-      </c>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="10">
-        <v>81.900000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="10">
-        <v>55.9</v>
-      </c>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="10">
-        <v>89.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A336C0-003C-4732-B650-95E6988755F8}">
-  <dimension ref="B2:K21"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -862,7 +628,10 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <f t="array" ref="D7">INDEX($I$7:$K$21,MATCH(B7&amp;C7,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>89.99</v>
+      </c>
       <c r="I7" s="9" t="s">
         <v>3</v>
       </c>
@@ -880,7 +649,10 @@
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7">
+        <f t="array" ref="D8">INDEX($I$7:$K$21,MATCH(B8&amp;C8,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>148.56</v>
+      </c>
       <c r="I8" s="9" t="s">
         <v>3</v>
       </c>
@@ -898,7 +670,10 @@
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7">
+        <f t="array" ref="D9">INDEX($I$7:$K$21,MATCH(B9&amp;C9,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>46.9</v>
+      </c>
       <c r="I9" s="9" t="s">
         <v>16</v>
       </c>
@@ -916,7 +691,275 @@
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7">
+        <f t="array" ref="D10">INDEX($I$7:$K$21,MATCH(B10&amp;C10,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>69.989999999999995</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="10">
+        <v>148.56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="10">
+        <v>146.13999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="10">
+        <v>224.14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="10">
+        <v>150.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="10">
+        <v>248.73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="10">
+        <v>116.52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="10">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="10">
+        <v>46.9</v>
+      </c>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="10">
+        <v>41.9</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="10">
+        <v>81.900000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="10">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="10">
+        <v>89.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A336C0-003C-4732-B650-95E6988755F8}">
+  <dimension ref="B2:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" cm="1">
+        <f t="array" ref="D7">INDEX(I7:K21,MATCH(B7&amp;C7,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>89.99</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="10">
+        <v>89.99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="7" cm="1">
+        <f t="array" ref="D8">INDEX(I8:K22,MATCH(B8&amp;C8,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>146.13999999999999</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="10">
+        <v>69.989999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" cm="1">
+        <f t="array" ref="D9">INDEX(I9:K23,MATCH(B9&amp;C9,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>81.900000000000006</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="10">
+        <v>153.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" cm="1">
+        <f t="array" ref="D10">INDEX(I10:K24,MATCH(B10&amp;C10,$I$7:$I$21&amp;$J$7:$J$21,0),3)</f>
+        <v>146.13999999999999</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>12</v>
       </c>

</xml_diff>